<commit_message>
modification plan effectif #4
</commit_message>
<xml_diff>
--- a/Documentation/planEffectif/PlanificationEffectif-TPI-Bonvallat-2021.xlsx
+++ b/Documentation/planEffectif/PlanificationEffectif-TPI-Bonvallat-2021.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17700"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17700"/>
   </bookViews>
   <sheets>
     <sheet name="Votre feuille" sheetId="1" r:id="rId1"/>
@@ -1012,7 +1012,7 @@
   <dimension ref="A1:AA1004"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1343,7 +1343,9 @@
       <c r="B14" s="24">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="D14" s="11"/>
+      <c r="D14" s="11">
+        <v>0.125</v>
+      </c>
       <c r="E14" s="21"/>
       <c r="F14" s="11"/>
       <c r="G14" s="21"/>
@@ -1355,7 +1357,7 @@
       <c r="M14" s="15"/>
       <c r="N14" s="11">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.125</v>
       </c>
     </row>
     <row r="15" spans="1:27">
@@ -1767,7 +1769,7 @@
       </c>
       <c r="D33" s="11">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>0.125</v>
       </c>
       <c r="E33" s="11">
         <f t="shared" si="2"/>
@@ -1809,11 +1811,11 @@
     <row r="34" spans="2:14" ht="15.75" customHeight="1">
       <c r="M34" s="11">
         <f>SUM(C33:M33)</f>
-        <v>0.37500000000000006</v>
+        <v>0.5</v>
       </c>
       <c r="N34" s="11">
         <f>SUM(N2:N32)</f>
-        <v>0.37500000000000006</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="35" spans="2:14" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
mise a jour plan effectif #4
</commit_message>
<xml_diff>
--- a/Documentation/planEffectif/PlanificationEffectif-TPI-Bonvallat-2021.xlsx
+++ b/Documentation/planEffectif/PlanificationEffectif-TPI-Bonvallat-2021.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17700"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17700"/>
   </bookViews>
   <sheets>
     <sheet name="Votre feuille" sheetId="1" r:id="rId1"/>
@@ -1012,7 +1012,7 @@
   <dimension ref="A1:AA1004"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="J38" sqref="J38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1368,7 +1368,9 @@
         <v>0.20833333333333334</v>
       </c>
       <c r="C15" s="21"/>
-      <c r="D15" s="11"/>
+      <c r="D15" s="11">
+        <v>0.25</v>
+      </c>
       <c r="E15" s="14"/>
       <c r="F15" s="11"/>
       <c r="G15" s="21"/>
@@ -1380,7 +1382,7 @@
       <c r="M15" s="15"/>
       <c r="N15" s="11">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="16" spans="1:27">
@@ -1687,7 +1689,9 @@
       <c r="C29" s="14">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="D29" s="14"/>
+      <c r="D29" s="14">
+        <v>8.3333333333333329E-2</v>
+      </c>
       <c r="E29" s="14"/>
       <c r="F29" s="14"/>
       <c r="G29" s="14"/>
@@ -1699,7 +1703,7 @@
       <c r="M29" s="14"/>
       <c r="N29" s="11">
         <f>SUM(C29:M29)</f>
-        <v>4.1666666666666664E-2</v>
+        <v>0.125</v>
       </c>
     </row>
     <row r="30" spans="1:14" ht="15.75" customHeight="1">
@@ -1769,7 +1773,7 @@
       </c>
       <c r="D33" s="11">
         <f t="shared" si="2"/>
-        <v>0.125</v>
+        <v>0.45833333333333331</v>
       </c>
       <c r="E33" s="11">
         <f t="shared" si="2"/>
@@ -1811,11 +1815,11 @@
     <row r="34" spans="2:14" ht="15.75" customHeight="1">
       <c r="M34" s="11">
         <f>SUM(C33:M33)</f>
-        <v>0.5</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="N34" s="11">
         <f>SUM(N2:N32)</f>
-        <v>0.5</v>
+        <v>0.83333333333333337</v>
       </c>
     </row>
     <row r="35" spans="2:14" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
mise a jour plan prévisionnel
Après-midi 5e jour
</commit_message>
<xml_diff>
--- a/Documentation/planEffectif/PlanificationEffectif-TPI-Bonvallat-2021.xlsx
+++ b/Documentation/planEffectif/PlanificationEffectif-TPI-Bonvallat-2021.xlsx
@@ -1017,7 +1017,7 @@
   <dimension ref="A1:AA1004"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1496,7 +1496,9 @@
       <c r="D20" s="11"/>
       <c r="E20" s="14"/>
       <c r="F20" s="11"/>
-      <c r="G20" s="14"/>
+      <c r="G20" s="14">
+        <v>0.125</v>
+      </c>
       <c r="H20" s="11"/>
       <c r="I20" s="14"/>
       <c r="J20" s="14"/>
@@ -1505,7 +1507,7 @@
       <c r="M20" s="15"/>
       <c r="N20" s="11">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.125</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
@@ -1563,7 +1565,9 @@
       <c r="D23" s="11"/>
       <c r="E23" s="14"/>
       <c r="F23" s="11"/>
-      <c r="G23" s="14"/>
+      <c r="G23" s="14">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="H23" s="11"/>
       <c r="J23" s="14"/>
       <c r="K23" s="11"/>
@@ -1571,7 +1575,7 @@
       <c r="M23" s="50"/>
       <c r="N23" s="11">
         <f>SUM(C23:M23)</f>
-        <v>0</v>
+        <v>4.1666666666666664E-2</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
@@ -1655,7 +1659,9 @@
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="F27" s="11"/>
-      <c r="G27" s="11"/>
+      <c r="G27" s="11">
+        <v>0.125</v>
+      </c>
       <c r="H27" s="11"/>
       <c r="I27" s="11"/>
       <c r="J27" s="11"/>
@@ -1664,7 +1670,7 @@
       <c r="M27" s="11"/>
       <c r="N27" s="11">
         <f>SUM(C27:M27)</f>
-        <v>0.16666666666666666</v>
+        <v>0.29166666666666663</v>
       </c>
     </row>
     <row r="28" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1709,7 +1715,9 @@
       <c r="F29" s="14">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="G29" s="14"/>
+      <c r="G29" s="14">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="H29" s="14"/>
       <c r="I29" s="14"/>
       <c r="J29" s="14"/>
@@ -1718,7 +1726,7 @@
       <c r="M29" s="14"/>
       <c r="N29" s="11">
         <f>SUM(C29:M29)</f>
-        <v>0.24999999999999997</v>
+        <v>0.29166666666666663</v>
       </c>
     </row>
     <row r="30" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1800,7 +1808,7 @@
       </c>
       <c r="G33" s="11">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="H33" s="11">
         <f t="shared" si="2"/>
@@ -1830,11 +1838,11 @@
     <row r="34" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="M34" s="11">
         <f>SUM(C33:M33)</f>
-        <v>1.3541666666666667</v>
+        <v>1.6875</v>
       </c>
       <c r="N34" s="11">
         <f>SUM(N2:N32)</f>
-        <v>1.3541666666666667</v>
+        <v>1.6875</v>
       </c>
     </row>
     <row r="35" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>